<commit_message>
fix the excel sheet name and adding five virus analysis
</commit_message>
<xml_diff>
--- a/celegans.fasta_slected.xlsx
+++ b/celegans.fasta_slected.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ltao/gitsss/de-enrichemnt-analysis/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D59D94A-4313-8545-9233-208269980A06}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="1080" yWindow="460" windowWidth="23660" windowHeight="11380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="D_E40_70" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -526,8 +532,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -590,6 +596,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -636,7 +650,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -668,9 +682,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -702,6 +734,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -877,14 +927,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="255.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="146.6640625" customWidth="1"/>
+    <col min="8" max="8" width="5.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -907,7 +965,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -933,7 +991,7 @@
         <v>1538</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -959,7 +1017,7 @@
         <v>2392</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -985,7 +1043,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -1011,7 +1069,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -1037,7 +1095,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -1063,7 +1121,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -1089,7 +1147,7 @@
         <v>1705</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
@@ -1115,7 +1173,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
@@ -1141,7 +1199,7 @@
         <v>1778</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
@@ -1167,7 +1225,7 @@
         <v>2493</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
@@ -1193,7 +1251,7 @@
         <v>2491</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
@@ -1219,7 +1277,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
@@ -1245,7 +1303,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>20</v>
       </c>
@@ -1271,7 +1329,7 @@
         <v>2493</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>21</v>
       </c>
@@ -1297,7 +1355,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>22</v>
       </c>
@@ -1323,7 +1381,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>23</v>
       </c>
@@ -1349,7 +1407,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>24</v>
       </c>
@@ -1375,7 +1433,7 @@
         <v>3769</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>25</v>
       </c>
@@ -1401,7 +1459,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>26</v>
       </c>
@@ -1427,7 +1485,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>27</v>
       </c>
@@ -1453,7 +1511,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>28</v>
       </c>
@@ -1479,7 +1537,7 @@
         <v>1061</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>29</v>
       </c>
@@ -1505,7 +1563,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>30</v>
       </c>
@@ -1531,7 +1589,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>31</v>
       </c>
@@ -1557,7 +1615,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>32</v>
       </c>
@@ -1583,7 +1641,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>33</v>
       </c>
@@ -1609,7 +1667,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>34</v>
       </c>
@@ -1635,7 +1693,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>35</v>
       </c>
@@ -1661,7 +1719,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>36</v>
       </c>
@@ -1687,7 +1745,7 @@
         <v>2491</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>37</v>
       </c>
@@ -1713,7 +1771,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>38</v>
       </c>
@@ -1739,7 +1797,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>39</v>
       </c>
@@ -1765,7 +1823,7 @@
         <v>2493</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>40</v>
       </c>
@@ -1791,7 +1849,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>41</v>
       </c>
@@ -1817,7 +1875,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>42</v>
       </c>
@@ -1843,7 +1901,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>43</v>
       </c>
@@ -1869,7 +1927,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>44</v>
       </c>
@@ -1895,7 +1953,7 @@
         <v>2491</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>45</v>
       </c>
@@ -1921,7 +1979,7 @@
         <v>1783</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>46</v>
       </c>
@@ -1947,7 +2005,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>47</v>
       </c>
@@ -1973,7 +2031,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>48</v>
       </c>
@@ -1999,7 +2057,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>49</v>
       </c>
@@ -2025,7 +2083,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>50</v>
       </c>
@@ -2051,7 +2109,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>51</v>
       </c>
@@ -2077,7 +2135,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>52</v>
       </c>
@@ -2103,7 +2161,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>53</v>
       </c>
@@ -2129,7 +2187,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>54</v>
       </c>
@@ -2155,7 +2213,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>55</v>
       </c>
@@ -2181,7 +2239,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>56</v>
       </c>
@@ -2207,7 +2265,7 @@
         <v>843</v>
       </c>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>57</v>
       </c>
@@ -2233,7 +2291,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>58</v>
       </c>
@@ -2259,7 +2317,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>59</v>
       </c>
@@ -2285,7 +2343,7 @@
         <v>1352</v>
       </c>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>60</v>
       </c>
@@ -2311,7 +2369,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>61</v>
       </c>
@@ -2337,7 +2395,7 @@
         <v>2491</v>
       </c>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>62</v>
       </c>
@@ -2363,7 +2421,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>63</v>
       </c>

</xml_diff>